<commit_message>
Modify BuildingInfo.xlsx (add data about Sprint2)
</commit_message>
<xml_diff>
--- a/BuildingInfo.xlsx
+++ b/BuildingInfo.xlsx
@@ -5,28 +5,21 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kubi\Desktop\PUT_term5_IO_BuildingInfo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\48724\Documents\GitHub\PUT_term5_IO_BuildingInfo2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C98BF6F7-F406-4A75-B320-2E869E621E6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F052D38A-E125-4ADA-98FB-113A3C4A9F13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="1140" windowWidth="22425" windowHeight="14100" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-13068" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Opis" sheetId="3" r:id="rId1"/>
     <sheet name="Product Backlog" sheetId="1" r:id="rId2"/>
     <sheet name="Sprint Backlog #1" sheetId="2" r:id="rId3"/>
+    <sheet name="Sprint Backlog #2" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -35,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="56">
   <si>
     <t>Element rejestru produktu</t>
   </si>
@@ -217,6 +210,27 @@
   </si>
   <si>
     <t>Jako zarządca budynku mogę sprawdzić listę pokoi o powierzchni większej lub równej od zadanej wartości</t>
+  </si>
+  <si>
+    <t>Funkcjonalność zwracająca czynsz dla pomieszczenia</t>
+  </si>
+  <si>
+    <t>Funkcjonalność zwracająca czynsz dla poziomu</t>
+  </si>
+  <si>
+    <t>Funkcjonalność zwracająca czynsz dla budynku</t>
+  </si>
+  <si>
+    <t>Funkcjonalność zwracająca listę pokoi o czynszach nie większych niż zadany na poziomie</t>
+  </si>
+  <si>
+    <t>Funkcjonalność łącząca listy pokoi o czynszach nie większych niż zadany na poszczególnych poziomach w jedną listę</t>
+  </si>
+  <si>
+    <t>Funkcjonalność zwracająca wygenerowaną listę</t>
+  </si>
+  <si>
+    <t>Funkcjonalność licząca zużycie energii na ogrzewanie</t>
   </si>
 </sst>
 </file>
@@ -536,7 +550,39 @@
     <cellStyle name="Odwiedzone hiperłącze" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Odwiedzone hiperłącze" xfId="18" builtinId="9" hidden="1"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="14">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
     </dxf>
@@ -611,26 +657,38 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela2" displayName="Tabela2" ref="A1:E8" totalsRowShown="0" headerRowDxfId="9">
-  <autoFilter ref="A1:E8" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela2" displayName="Tabela2" ref="A1:E11" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="A1:E11" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Element rejestru produktu" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Ważność" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Pracochłonność" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Business Value (BV)" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Kryteria akceptacji" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Element rejestru produktu" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Ważność" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Pracochłonność" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Business Value (BV)" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Kryteria akceptacji" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabela3" displayName="Tabela3" ref="A4:C48" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabela3" displayName="Tabela3" ref="A4:C48" totalsRowShown="0" headerRowDxfId="7">
   <autoFilter ref="A4:C48" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Element rejestru produktu" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Zadania" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Pracochłonność " dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Element rejestru produktu" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Zadania" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Pracochłonność " dataDxfId="4"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EC1E0423-8B61-4F9A-BF5C-FB702E030AAC}" name="Tabela32" displayName="Tabela32" ref="A1:C35" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A1:C35" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{E98E85F4-43C9-4B3D-B8DA-10871119C156}" name="Element rejestru produktu" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{A604E83F-FA48-4170-8B60-AA629B00AEBB}" name="Zadania" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{BA30B065-E778-49ED-88B8-5D2EFEAFA4F8}" name="Pracochłonność " dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -964,22 +1022,22 @@
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="95.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="85.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="189" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
@@ -996,22 +1054,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="52" style="3" customWidth="1"/>
     <col min="2" max="2" width="15" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="58.25" style="3" customWidth="1"/>
+    <col min="3" max="3" width="21.69921875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.19921875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="58.19921875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1028,7 +1086,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
@@ -1045,7 +1103,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="78" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
@@ -1062,7 +1120,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="78" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
@@ -1079,7 +1137,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
@@ -1096,13 +1154,16 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="4">
         <v>10</v>
       </c>
+      <c r="C6" s="4">
+        <v>7</v>
+      </c>
       <c r="D6" s="4">
         <v>1</v>
       </c>
@@ -1110,65 +1171,86 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="B7" s="4">
         <v>10</v>
       </c>
+      <c r="C7" s="4">
+        <v>7</v>
+      </c>
       <c r="D7" s="4">
+        <v>1</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="4">
+        <v>10</v>
+      </c>
+      <c r="C8" s="4">
+        <v>7</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="78" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="4">
+        <v>10</v>
+      </c>
+      <c r="D10" s="4">
         <v>1.5</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+    <row r="11" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="D11" s="4">
+        <v>2</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+    <row r="12" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E12" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="63" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+    <row r="13" spans="1:5" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E13" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E15" s="3" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1188,25 +1270,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:C22"/>
+  <dimension ref="A2:C24"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45.25" style="3" customWidth="1"/>
-    <col min="2" max="2" width="70.125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="45.19921875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="70.09765625" style="3" customWidth="1"/>
     <col min="3" max="3" width="33" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
         <v>0</v>
       </c>
@@ -1217,7 +1299,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>12</v>
       </c>
@@ -1226,7 +1308,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="9"/>
       <c r="B6" s="11" t="s">
         <v>25</v>
@@ -1235,7 +1317,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="9"/>
       <c r="B7" s="11" t="s">
         <v>26</v>
@@ -1244,7 +1326,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="9"/>
       <c r="B8" s="13" t="s">
         <v>27</v>
@@ -1253,7 +1335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="9"/>
       <c r="B9" s="11" t="s">
         <v>28</v>
@@ -1262,7 +1344,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="14"/>
       <c r="B10" s="12" t="s">
         <v>29</v>
@@ -1271,7 +1353,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>14</v>
       </c>
@@ -1280,7 +1362,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="9"/>
       <c r="B12" s="15" t="s">
         <v>30</v>
@@ -1289,7 +1371,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="9"/>
       <c r="B13" s="15" t="s">
         <v>31</v>
@@ -1298,7 +1380,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="10"/>
       <c r="B14" s="15" t="s">
         <v>32</v>
@@ -1307,7 +1389,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="78" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>16</v>
       </c>
@@ -1316,7 +1398,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="9"/>
       <c r="B16" s="15" t="s">
         <v>33</v>
@@ -1325,7 +1407,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="9"/>
       <c r="B17" s="15" t="s">
         <v>34</v>
@@ -1334,7 +1416,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="10"/>
       <c r="B18" s="15" t="s">
         <v>35</v>
@@ -1343,7 +1425,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
         <v>18</v>
       </c>
@@ -1352,7 +1434,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="9"/>
       <c r="B20" s="15" t="s">
         <v>36</v>
@@ -1361,7 +1443,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="9"/>
       <c r="B21" s="15" t="s">
         <v>37</v>
@@ -1370,13 +1452,31 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="10"/>
       <c r="B22" s="15" t="s">
         <v>38</v>
       </c>
       <c r="C22" s="20">
         <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="9"/>
+      <c r="C23" s="16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="9"/>
+      <c r="B24" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="20">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1391,4 +1491,111 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FEDC7F0-8262-4720-A222-5E00EA84ACCA}">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="45.19921875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="97.3984375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="33" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="9"/>
+      <c r="B3" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="9"/>
+      <c r="B4" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="10"/>
+      <c r="B5" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="9"/>
+      <c r="B7" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="9"/>
+      <c r="B8" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="10"/>
+      <c r="B9" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="20">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>